<commit_message>
Changed code to generalize station name (station and alternative station name). Changed excel files to be compatible (added NEW STATION column to those without it).
</commit_message>
<xml_diff>
--- a/data/nc/conditional_sampling_ncdmf/datasheets/cond_a2.xlsx
+++ b/data/nc/conditional_sampling_ncdmf/datasheets/cond_a2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahaines\Desktop\Method Comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megancarr/Documents/data_analytics_research/shellbase_with_usc/data/nc/conditional_sampling_ncdmf/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E80987-8F72-DB4B-8EBE-E1254A93A510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>STATION</t>
   </si>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -239,6 +240,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -274,6 +292,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -449,25 +484,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:MB84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="LR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="MB6" sqref="MB6"/>
+      <pane xSplit="3" topLeftCell="LX1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="10"/>
+    <col min="1" max="1" width="10.85546875" style="10"/>
     <col min="2" max="2" width="11" style="4" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" style="7" customWidth="1"/>
-    <col min="4" max="135" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="8.33203125" style="7" customWidth="1"/>
-    <col min="137" max="16384" width="10.88671875" style="7"/>
+    <col min="3" max="3" width="4.140625" style="7" customWidth="1"/>
+    <col min="4" max="135" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="8.28515625" style="7" customWidth="1"/>
+    <col min="137" max="16384" width="10.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:340" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:340" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1524,7 @@
         <v>44180</v>
       </c>
     </row>
-    <row r="2" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
@@ -1647,7 +1682,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="3" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -2384,7 +2419,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
@@ -2752,7 +2787,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
@@ -2943,7 +2978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -3059,7 +3094,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -3103,11 +3138,13 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="LV8" s="5">
         <v>130</v>
       </c>
@@ -3115,7 +3152,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="9" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -3357,7 +3394,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9"/>
       <c r="B10" s="4">
         <v>13</v>
@@ -3581,7 +3618,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9"/>
       <c r="B11" s="4">
         <v>7</v>
@@ -4229,7 +4266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
       <c r="B12" s="4">
         <v>6</v>
@@ -4418,7 +4455,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="13" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="4">
         <v>10</v>
@@ -4778,7 +4815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="4">
         <v>20</v>
@@ -4940,7 +4977,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="15" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="4">
         <v>11</v>
@@ -5240,7 +5277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:340" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="4">
         <v>20</v>
@@ -5429,7 +5466,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="4">
         <v>8</v>
@@ -5552,7 +5589,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="18" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="4">
         <v>17</v>
@@ -5570,7 +5607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
       <c r="B19" s="4" t="s">
         <v>2</v>
@@ -5579,7 +5616,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="20" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9"/>
       <c r="B20" s="4">
         <v>16</v>
@@ -5588,7 +5625,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9"/>
       <c r="B21" s="4" t="s">
         <v>4</v>
@@ -5600,7 +5637,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="22" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9"/>
       <c r="B22" s="4">
         <v>5</v>
@@ -5612,7 +5649,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9"/>
       <c r="B23" s="4">
         <v>14</v>
@@ -5624,43 +5661,43 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9"/>
       <c r="B24" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9"/>
       <c r="B25" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="B26" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9"/>
       <c r="B27" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9"/>
       <c r="B28" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9"/>
       <c r="B29" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9"/>
       <c r="B30" s="4">
         <v>20</v>
@@ -5675,7 +5712,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
@@ -5777,7 +5814,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9"/>
       <c r="B32" s="4" t="s">
         <v>6</v>
@@ -5786,7 +5823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="4">
         <v>18</v>
@@ -5795,212 +5832,212 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9"/>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="9"/>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="9"/>
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="9"/>
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="9"/>
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="9"/>
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A46" s="9"/>
       <c r="B46" s="4"/>
     </row>
-    <row r="47" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="9"/>
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:273" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="9"/>
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A49" s="9"/>
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A50" s="9"/>
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A51" s="9"/>
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A52" s="9"/>
       <c r="B52" s="4"/>
     </row>
-    <row r="53" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A53" s="9"/>
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="9"/>
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A55" s="9"/>
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="9"/>
       <c r="B56" s="4"/>
     </row>
-    <row r="57" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A57" s="9"/>
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A58" s="9"/>
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A59" s="9"/>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A60" s="9"/>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A61" s="9"/>
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A62" s="9"/>
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A63" s="9"/>
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A64" s="9"/>
       <c r="B64" s="4"/>
     </row>
-    <row r="65" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A65" s="9"/>
       <c r="B65" s="4"/>
     </row>
-    <row r="66" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A66" s="9"/>
       <c r="B66" s="4"/>
     </row>
-    <row r="67" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A67" s="9"/>
       <c r="B67" s="4"/>
     </row>
-    <row r="68" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A68" s="9"/>
       <c r="B68" s="4"/>
     </row>
-    <row r="69" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A69" s="9"/>
       <c r="B69" s="4"/>
     </row>
-    <row r="70" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A70" s="9"/>
       <c r="B70" s="4"/>
     </row>
-    <row r="71" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A71" s="9"/>
       <c r="B71" s="4"/>
     </row>
-    <row r="72" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A72" s="9"/>
       <c r="B72" s="4"/>
     </row>
-    <row r="73" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A73" s="9"/>
       <c r="B73" s="4"/>
     </row>
-    <row r="74" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A74" s="9"/>
       <c r="B74" s="4"/>
     </row>
-    <row r="75" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A75" s="9"/>
       <c r="B75" s="4"/>
     </row>
-    <row r="76" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A76" s="9"/>
       <c r="B76" s="4"/>
     </row>
-    <row r="77" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A77" s="9"/>
       <c r="B77" s="4"/>
     </row>
-    <row r="78" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A78" s="9"/>
       <c r="B78" s="4"/>
     </row>
-    <row r="79" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A79" s="9"/>
       <c r="B79" s="4"/>
     </row>
-    <row r="80" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A80" s="9"/>
       <c r="B80" s="4"/>
     </row>
-    <row r="81" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A81" s="9"/>
       <c r="B81" s="4"/>
     </row>
-    <row r="82" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A82" s="9"/>
       <c r="B82" s="4"/>
     </row>
-    <row r="83" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A83" s="9"/>
       <c r="B83" s="4"/>
     </row>
-    <row r="84" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A84" s="9"/>
       <c r="B84" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:KD83">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:KD83">
     <sortCondition ref="A2:A83"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>